<commit_message>
Daily push for 20200618
</commit_message>
<xml_diff>
--- a/Graphics/20200618/20200618_Kosovo_COVID.xlsx
+++ b/Graphics/20200618/20200618_Kosovo_COVID.xlsx
@@ -478,61 +478,61 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F2" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H2" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I2" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J2" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K2" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L2" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M2" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N2" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O2" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P2" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q2" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="R2" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S2" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="T2" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3">
@@ -542,61 +542,61 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>290.5333333333334</v>
+        <v>296.0714285714286</v>
       </c>
       <c r="C3" t="n">
-        <v>51.6</v>
+        <v>49.35714285714285</v>
       </c>
       <c r="D3" t="n">
-        <v>8.4</v>
+        <v>6.928571428571429</v>
       </c>
       <c r="E3" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="F3" t="n">
-        <v>27.4</v>
+        <v>29.14285714285714</v>
       </c>
       <c r="G3" t="n">
-        <v>17503</v>
+        <v>17642.85714285714</v>
       </c>
       <c r="H3" t="n">
-        <v>0.07716380880017286</v>
+        <v>0.0676665693209533</v>
       </c>
       <c r="I3" t="n">
-        <v>1373.733333333333</v>
+        <v>1385.714285714286</v>
       </c>
       <c r="J3" t="n">
-        <v>0.5783138773568368</v>
+        <v>0.5542334992567309</v>
       </c>
       <c r="K3" t="n">
-        <v>917.2666666666667</v>
+        <v>920.2142857142857</v>
       </c>
       <c r="L3" t="n">
-        <v>1.04531746031746</v>
+        <v>0.6914115646258503</v>
       </c>
       <c r="M3" t="n">
-        <v>31.6</v>
+        <v>31.64285714285714</v>
       </c>
       <c r="N3" t="n">
-        <v>-0.1333333333333333</v>
+        <v>-0.2142857142857143</v>
       </c>
       <c r="O3" t="n">
-        <v>1518.2</v>
+        <v>1528.857142857143</v>
       </c>
       <c r="P3" t="n">
-        <v>0.1459425092048551</v>
+        <v>0.1644532275173312</v>
       </c>
       <c r="Q3" t="n">
-        <v>16.47229156286535</v>
+        <v>15.83416118027548</v>
       </c>
       <c r="R3" t="n">
-        <v>424.8666666666667</v>
+        <v>433.8571428571428</v>
       </c>
       <c r="S3" t="n">
-        <v>47.33333333333334</v>
+        <v>47.28571428571428</v>
       </c>
       <c r="T3" t="n">
-        <v>43.37777777777777</v>
+        <v>43.54761904761904</v>
       </c>
     </row>
     <row r="4">
@@ -606,61 +606,61 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>62.03324761387081</v>
+        <v>69.14473592034686</v>
       </c>
       <c r="C4" t="n">
-        <v>47.01337195795621</v>
+        <v>41.5684924003693</v>
       </c>
       <c r="D4" t="n">
-        <v>8.466741656960741</v>
+        <v>7.790174143548602</v>
       </c>
       <c r="E4" t="n">
-        <v>0.4879500364742667</v>
+        <v>0.4688072309384954</v>
       </c>
       <c r="F4" t="n">
-        <v>16.81326007310047</v>
+        <v>17.36423000067908</v>
       </c>
       <c r="G4" t="n">
-        <v>1259.478236640645</v>
+        <v>1190.733184421899</v>
       </c>
       <c r="H4" t="n">
-        <v>0.2527021881844064</v>
+        <v>0.253093697129491</v>
       </c>
       <c r="I4" t="n">
-        <v>228.2825525736118</v>
+        <v>216.7928570251863</v>
       </c>
       <c r="J4" t="n">
-        <v>1.241900978992929</v>
+        <v>1.309777373697728</v>
       </c>
       <c r="K4" t="n">
-        <v>34.6728932137127</v>
+        <v>32.85908976553946</v>
       </c>
       <c r="L4" t="n">
-        <v>2.447772503836224</v>
+        <v>2.313503716417428</v>
       </c>
       <c r="M4" t="n">
-        <v>1.502379065729703</v>
+        <v>1.336306209562122</v>
       </c>
       <c r="N4" t="n">
-        <v>0.3518657752744984</v>
+        <v>0.42581531362632</v>
       </c>
       <c r="O4" t="n">
-        <v>129.0897804962555</v>
+        <v>128.4055217737073</v>
       </c>
       <c r="P4" t="n">
-        <v>0.2421071118489106</v>
+        <v>0.2440520188195535</v>
       </c>
       <c r="Q4" t="n">
-        <v>11.50524522595199</v>
+        <v>10.39897970898935</v>
       </c>
       <c r="R4" t="n">
-        <v>194.3464750926869</v>
+        <v>184.6772057663596</v>
       </c>
       <c r="S4" t="n">
-        <v>42.27954025068772</v>
+        <v>38.30380292714182</v>
       </c>
       <c r="T4" t="n">
-        <v>36.6484514639977</v>
+        <v>33.62859160568836</v>
       </c>
     </row>
     <row r="5">
@@ -685,19 +685,19 @@
         <v>9</v>
       </c>
       <c r="G5" t="n">
-        <v>15585</v>
+        <v>15879</v>
       </c>
       <c r="H5" t="n">
         <v>-0.3232323232323232</v>
       </c>
       <c r="I5" t="n">
-        <v>1142</v>
+        <v>1147</v>
       </c>
       <c r="J5" t="n">
         <v>-0.7931034482758621</v>
       </c>
       <c r="K5" t="n">
-        <v>871</v>
+        <v>874</v>
       </c>
       <c r="L5" t="n">
         <v>-1</v>
@@ -709,7 +709,7 @@
         <v>-1</v>
       </c>
       <c r="O5" t="n">
-        <v>1375</v>
+        <v>1384</v>
       </c>
       <c r="P5" t="n">
         <v>-0.09677419354838712</v>
@@ -718,7 +718,7 @@
         <v>1.700680272108844</v>
       </c>
       <c r="R5" t="n">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="S5" t="n">
         <v>8</v>
@@ -734,37 +734,37 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>242</v>
+        <v>239.5</v>
       </c>
       <c r="C6" t="n">
-        <v>23.5</v>
+        <v>28.25</v>
       </c>
       <c r="D6" t="n">
-        <v>2.5</v>
+        <v>1.25</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>11</v>
+        <v>13.25</v>
       </c>
       <c r="G6" t="n">
-        <v>16525</v>
+        <v>16730.75</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.1004868401034535</v>
+        <v>-0.1269207363456565</v>
       </c>
       <c r="I6" t="n">
-        <v>1214</v>
+        <v>1241.25</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.08083929733246581</v>
+        <v>-0.227801724137931</v>
       </c>
       <c r="K6" t="n">
-        <v>887</v>
+        <v>895.5</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.55</v>
+        <v>-0.80625</v>
       </c>
       <c r="M6" t="n">
         <v>31</v>
@@ -773,22 +773,22 @@
         <v>0</v>
       </c>
       <c r="O6" t="n">
-        <v>1411.5</v>
+        <v>1422</v>
       </c>
       <c r="P6" t="n">
         <v>0</v>
       </c>
       <c r="Q6" t="n">
-        <v>8.93351214003388</v>
+        <v>10.83803258145363</v>
       </c>
       <c r="R6" t="n">
-        <v>296</v>
+        <v>314.75</v>
       </c>
       <c r="S6" t="n">
-        <v>17.5</v>
+        <v>19</v>
       </c>
       <c r="T6" t="n">
-        <v>20.33333333333334</v>
+        <v>21.08333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -801,34 +801,34 @@
         <v>294</v>
       </c>
       <c r="C7" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D7" t="n">
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>23</v>
+        <v>25.5</v>
       </c>
       <c r="G7" t="n">
-        <v>17478</v>
+        <v>17592</v>
       </c>
       <c r="H7" t="n">
-        <v>0.01020408163265296</v>
+        <v>0.02068645640074207</v>
       </c>
       <c r="I7" t="n">
-        <v>1298</v>
+        <v>1312</v>
       </c>
       <c r="J7" t="n">
-        <v>0.09302325581395343</v>
+        <v>0.02927024859663191</v>
       </c>
       <c r="K7" t="n">
-        <v>913</v>
+        <v>917</v>
       </c>
       <c r="L7" t="n">
-        <v>0</v>
+        <v>-0.2916666666666667</v>
       </c>
       <c r="M7" t="n">
         <v>31</v>
@@ -837,22 +837,22 @@
         <v>0</v>
       </c>
       <c r="O7" t="n">
-        <v>1483</v>
+        <v>1498.5</v>
       </c>
       <c r="P7" t="n">
-        <v>0</v>
+        <v>0.128032345013477</v>
       </c>
       <c r="Q7" t="n">
-        <v>13.51351351351351</v>
+        <v>15.22321043087816</v>
       </c>
       <c r="R7" t="n">
-        <v>354</v>
+        <v>364</v>
       </c>
       <c r="S7" t="n">
-        <v>34.5</v>
+        <v>36.25</v>
       </c>
       <c r="T7" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8">
@@ -862,61 +862,61 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="C8" t="n">
-        <v>55.5</v>
+        <v>56.75</v>
       </c>
       <c r="D8" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="F8" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G8" t="n">
-        <v>18378.5</v>
+        <v>18444.75</v>
       </c>
       <c r="H8" t="n">
-        <v>0.2918040508714084</v>
+        <v>0.2450592885375494</v>
       </c>
       <c r="I8" t="n">
-        <v>1461.5</v>
+        <v>1473.75</v>
       </c>
       <c r="J8" t="n">
-        <v>1.135714285714286</v>
+        <v>1.167857142857143</v>
       </c>
       <c r="K8" t="n">
-        <v>940.5</v>
+        <v>946.75</v>
       </c>
       <c r="L8" t="n">
-        <v>2.619047619047619</v>
+        <v>1.928571428571429</v>
       </c>
       <c r="M8" t="n">
-        <v>32.5</v>
+        <v>32.75</v>
       </c>
       <c r="N8" t="n">
         <v>0</v>
       </c>
       <c r="O8" t="n">
-        <v>1594</v>
+        <v>1604</v>
       </c>
       <c r="P8" t="n">
-        <v>0.2361111111111112</v>
+        <v>0.2430555555555556</v>
       </c>
       <c r="Q8" t="n">
-        <v>22.0206134153437</v>
+        <v>18.34553646860039</v>
       </c>
       <c r="R8" t="n">
-        <v>488.5</v>
+        <v>494.25</v>
       </c>
       <c r="S8" t="n">
-        <v>53.25</v>
+        <v>54.375</v>
       </c>
       <c r="T8" t="n">
-        <v>49.83333333333334</v>
+        <v>51.58333333333334</v>
       </c>
     </row>
     <row r="9">
@@ -926,7 +926,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>397</v>
+        <v>437</v>
       </c>
       <c r="C9" t="n">
         <v>141</v>
@@ -938,34 +938,34 @@
         <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G9" t="n">
-        <v>19690</v>
+        <v>19730</v>
       </c>
       <c r="H9" t="n">
         <v>0.472636815920398</v>
       </c>
       <c r="I9" t="n">
-        <v>1897</v>
+        <v>1833</v>
       </c>
       <c r="J9" t="n">
         <v>3.833333333333333</v>
       </c>
       <c r="K9" t="n">
-        <v>973</v>
+        <v>968</v>
       </c>
       <c r="L9" t="n">
         <v>7</v>
       </c>
       <c r="M9" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N9" t="n">
         <v>0</v>
       </c>
       <c r="O9" t="n">
-        <v>1777</v>
+        <v>1783</v>
       </c>
       <c r="P9" t="n">
         <v>0.8181818181818181</v>
@@ -974,13 +974,13 @@
         <v>35.51637279596977</v>
       </c>
       <c r="R9" t="n">
-        <v>889</v>
+        <v>831</v>
       </c>
       <c r="S9" t="n">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="T9" t="n">
-        <v>137</v>
+        <v>115.6666666666667</v>
       </c>
     </row>
     <row r="10">
@@ -990,61 +990,61 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>3848.123809523809</v>
+        <v>4780.994505494505</v>
       </c>
       <c r="C10" t="n">
-        <v>2210.257142857143</v>
+        <v>1727.93956043956</v>
       </c>
       <c r="D10" t="n">
-        <v>71.6857142857143</v>
+        <v>60.68681318681319</v>
       </c>
       <c r="E10" t="n">
-        <v>0.2380952380952382</v>
+        <v>0.2197802197802198</v>
       </c>
       <c r="F10" t="n">
-        <v>282.6857142857143</v>
+        <v>301.5164835164835</v>
       </c>
       <c r="G10" t="n">
-        <v>1586285.428571429</v>
+        <v>1417845.516483516</v>
       </c>
       <c r="H10" t="n">
-        <v>0.06385839591318716</v>
+        <v>0.06405641952667454</v>
       </c>
       <c r="I10" t="n">
-        <v>52112.92380952381</v>
+        <v>46999.14285714286</v>
       </c>
       <c r="J10" t="n">
-        <v>1.542318041623594</v>
+        <v>1.715516768650519</v>
       </c>
       <c r="K10" t="n">
-        <v>1202.209523809524</v>
+        <v>1079.71978021978</v>
       </c>
       <c r="L10" t="n">
-        <v>5.991590230536657</v>
+        <v>5.352299445877252</v>
       </c>
       <c r="M10" t="n">
-        <v>2.257142857142857</v>
+        <v>1.785714285714286</v>
       </c>
       <c r="N10" t="n">
-        <v>0.1238095238095238</v>
+        <v>0.1813186813186813</v>
       </c>
       <c r="O10" t="n">
-        <v>16664.17142857143</v>
+        <v>16487.97802197802</v>
       </c>
       <c r="P10" t="n">
-        <v>0.0586158536078209</v>
+        <v>0.0595613878898997</v>
       </c>
       <c r="Q10" t="n">
-        <v>132.3706677092911</v>
+        <v>108.1387789879723</v>
       </c>
       <c r="R10" t="n">
-        <v>37770.55238095239</v>
+        <v>34105.67032967033</v>
       </c>
       <c r="S10" t="n">
-        <v>1787.559523809523</v>
+        <v>1467.181318681319</v>
       </c>
       <c r="T10" t="n">
-        <v>1343.108994708995</v>
+        <v>1130.882173382173</v>
       </c>
     </row>
     <row r="11">
@@ -1054,61 +1054,61 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.6104590239927008</v>
+        <v>0.7387428952807386</v>
       </c>
       <c r="C11" t="n">
-        <v>1.232393686553145</v>
+        <v>1.301420633390143</v>
       </c>
       <c r="D11" t="n">
-        <v>1.192885801004677</v>
+        <v>1.511427959212774</v>
       </c>
       <c r="E11" t="n">
-        <v>0.7882269819968922</v>
+        <v>1.066536450385077</v>
       </c>
       <c r="F11" t="n">
-        <v>0.6132662133020937</v>
+        <v>0.6137187429137952</v>
       </c>
       <c r="G11" t="n">
-        <v>0.1857427068676795</v>
+        <v>0.2323533105790927</v>
       </c>
       <c r="H11" t="n">
-        <v>0.1997053589757879</v>
+        <v>0.2797985951937662</v>
       </c>
       <c r="I11" t="n">
-        <v>1.171667676798271</v>
+        <v>0.9968608516171372</v>
       </c>
       <c r="J11" t="n">
-        <v>1.47135430022086</v>
+        <v>1.393962314916163</v>
       </c>
       <c r="K11" t="n">
-        <v>0.2739502682906428</v>
+        <v>0.1785215922666882</v>
       </c>
       <c r="L11" t="n">
-        <v>1.392082604961806</v>
+        <v>1.833273544762371</v>
       </c>
       <c r="M11" t="n">
-        <v>1.090772421416784</v>
+        <v>0.7713570612733985</v>
       </c>
       <c r="N11" t="n">
-        <v>-2.404763138710329</v>
+        <v>-1.565623981413945</v>
       </c>
       <c r="O11" t="n">
-        <v>0.7752858704365849</v>
+        <v>0.7433364698981577</v>
       </c>
       <c r="P11" t="n">
-        <v>1.697417493241809</v>
+        <v>1.576613262358033</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.5464234100978869</v>
+        <v>0.527238841766428</v>
       </c>
       <c r="R11" t="n">
-        <v>1.336239603367851</v>
+        <v>1.143659349855952</v>
       </c>
       <c r="S11" t="n">
-        <v>1.479177190545966</v>
+        <v>1.28170849888799</v>
       </c>
       <c r="T11" t="n">
-        <v>1.648473460893799</v>
+        <v>1.292041436307717</v>
       </c>
     </row>
     <row r="12">
@@ -1118,61 +1118,61 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.4469107771921719</v>
+        <v>-0.06270432000823156</v>
       </c>
       <c r="C12" t="n">
-        <v>0.2222034495981369</v>
+        <v>1.139702138063765</v>
       </c>
       <c r="D12" t="n">
-        <v>0.1903268110938825</v>
+        <v>1.719306494904817</v>
       </c>
       <c r="E12" t="n">
-        <v>-1.615384615384616</v>
+        <v>-1.034090909090909</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.8779960806548766</v>
+        <v>-0.8332831773326368</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.9703147322844803</v>
+        <v>-0.9393391866482568</v>
       </c>
       <c r="H12" t="n">
-        <v>-1.113192934487021</v>
+        <v>-0.9475210604080928</v>
       </c>
       <c r="I12" t="n">
-        <v>0.6540205842194027</v>
+        <v>0.03710262597958858</v>
       </c>
       <c r="J12" t="n">
-        <v>2.224204602134076</v>
+        <v>1.733023165910918</v>
       </c>
       <c r="K12" t="n">
-        <v>-1.103702031050164</v>
+        <v>-1.123453215190796</v>
       </c>
       <c r="L12" t="n">
-        <v>1.129883812023222</v>
+        <v>3.32622607722137</v>
       </c>
       <c r="M12" t="n">
-        <v>0.4387240703536133</v>
+        <v>-0.6054265734265711</v>
       </c>
       <c r="N12" t="n">
-        <v>4.349112426035501</v>
+        <v>0.5013774104683213</v>
       </c>
       <c r="O12" t="n">
-        <v>-0.518662163552456</v>
+        <v>-0.5409334097872081</v>
       </c>
       <c r="P12" t="n">
-        <v>3.282186473580841</v>
+        <v>3.025966364268879</v>
       </c>
       <c r="Q12" t="n">
-        <v>-0.7581506715242692</v>
+        <v>-0.1199902906939396</v>
       </c>
       <c r="R12" t="n">
-        <v>1.128863533419882</v>
+        <v>0.3826036335325655</v>
       </c>
       <c r="S12" t="n">
-        <v>1.253215324174565</v>
+        <v>0.8616806242548423</v>
       </c>
       <c r="T12" t="n">
-        <v>2.151214520240552</v>
+        <v>0.6545280671524933</v>
       </c>
     </row>
     <row r="13">
@@ -1182,61 +1182,61 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>46.49777777777778</v>
+        <v>49.80612244897959</v>
       </c>
       <c r="C13" t="n">
-        <v>35.2</v>
+        <v>30.1734693877551</v>
       </c>
       <c r="D13" t="n">
-        <v>6.320000000000001</v>
+        <v>5.489795918367347</v>
       </c>
       <c r="E13" t="n">
-        <v>0.4444444444444445</v>
+        <v>0.4081632653061224</v>
       </c>
       <c r="F13" t="n">
-        <v>13.62666666666667</v>
+        <v>13.87755102040816</v>
       </c>
       <c r="G13" t="n">
-        <v>1033.866666666667</v>
+        <v>973.5714285714286</v>
       </c>
       <c r="H13" t="n">
-        <v>0.211600295341395</v>
+        <v>0.2048372129180762</v>
       </c>
       <c r="I13" t="n">
-        <v>177.68</v>
+        <v>171.2040816326531</v>
       </c>
       <c r="J13" t="n">
-        <v>0.9491430469239311</v>
+        <v>1.034139248918573</v>
       </c>
       <c r="K13" t="n">
-        <v>27.48444444444444</v>
+        <v>25.78571428571428</v>
       </c>
       <c r="L13" t="n">
-        <v>2.001534391534391</v>
+        <v>1.781778425655976</v>
       </c>
       <c r="M13" t="n">
-        <v>1.2</v>
+        <v>1.112244897959183</v>
       </c>
       <c r="N13" t="n">
-        <v>0.2311111111111111</v>
+        <v>0.336734693877551</v>
       </c>
       <c r="O13" t="n">
-        <v>105.7066666666667</v>
+        <v>104.9795918367347</v>
       </c>
       <c r="P13" t="n">
-        <v>0.1783433429508575</v>
+        <v>0.1772805699677008</v>
       </c>
       <c r="Q13" t="n">
-        <v>9.082370679799981</v>
+        <v>7.812636754347187</v>
       </c>
       <c r="R13" t="n">
-        <v>149.5733333333333</v>
+        <v>144.530612244898</v>
       </c>
       <c r="S13" t="n">
-        <v>31.31111111111111</v>
+        <v>29.01020408163265</v>
       </c>
       <c r="T13" t="n">
-        <v>27.08148148148148</v>
+        <v>25.8469387755102</v>
       </c>
     </row>
   </sheetData>
@@ -1426,61 +1426,61 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>174.2477876106195</v>
+        <v>174.6017699115044</v>
       </c>
       <c r="C3" t="n">
-        <v>16.78761061946903</v>
+        <v>16.2212389380531</v>
       </c>
       <c r="D3" t="n">
-        <v>8.610619469026549</v>
+        <v>8.56637168141593</v>
       </c>
       <c r="E3" t="n">
-        <v>0.3097345132743363</v>
+        <v>0.3008849557522124</v>
       </c>
       <c r="F3" t="n">
-        <v>15.72566371681416</v>
+        <v>15.7787610619469</v>
       </c>
       <c r="G3" t="n">
-        <v>6923.743362831859</v>
+        <v>6924.097345132744</v>
       </c>
       <c r="H3" t="n">
-        <v>0.2917567582558344</v>
+        <v>0.2926484013311114</v>
       </c>
       <c r="I3" t="n">
-        <v>591.4601769911504</v>
+        <v>590.8938053097345</v>
       </c>
       <c r="J3" t="n">
-        <v>0.8885274662971482</v>
+        <v>0.8845106458615742</v>
       </c>
       <c r="K3" t="n">
-        <v>347.7433628318584</v>
+        <v>347.6991150442478</v>
       </c>
       <c r="L3" t="n">
-        <v>0.8282865921459815</v>
+        <v>0.8194370346238578</v>
       </c>
       <c r="M3" t="n">
-        <v>15.49557522123894</v>
+        <v>15.48672566371681</v>
       </c>
       <c r="N3" t="n">
-        <v>-0.1268436578171092</v>
+        <v>-0.135693215339233</v>
       </c>
       <c r="O3" t="n">
-        <v>630.8230088495575</v>
+        <v>630.8761061946902</v>
       </c>
       <c r="P3" t="n">
-        <v>0.01605126241546169</v>
+        <v>0.01705309911607949</v>
       </c>
       <c r="Q3" t="n">
-        <v>8.212313720747545</v>
+        <v>8.05393995529446</v>
       </c>
       <c r="R3" t="n">
-        <v>228.2212389380531</v>
+        <v>227.7079646017699</v>
       </c>
       <c r="S3" t="n">
-        <v>16.16371681415929</v>
+        <v>15.88053097345133</v>
       </c>
       <c r="T3" t="n">
-        <v>15.53982300884955</v>
+        <v>15.35103244837758</v>
       </c>
     </row>
     <row r="4">
@@ -1490,61 +1490,61 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>112.8464135588604</v>
+        <v>113.6115358063081</v>
       </c>
       <c r="C4" t="n">
-        <v>24.98515678194671</v>
+        <v>22.77166727743458</v>
       </c>
       <c r="D4" t="n">
-        <v>13.66462692784248</v>
+        <v>13.68450381831495</v>
       </c>
       <c r="E4" t="n">
-        <v>0.6557390326093796</v>
+        <v>0.6530827413152125</v>
       </c>
       <c r="F4" t="n">
-        <v>18.90495389895512</v>
+        <v>19.01866306762646</v>
       </c>
       <c r="G4" t="n">
-        <v>6310.449175741831</v>
+        <v>6311.172768483967</v>
       </c>
       <c r="H4" t="n">
-        <v>1.181888081950367</v>
+        <v>1.181704000650929</v>
       </c>
       <c r="I4" t="n">
-        <v>502.4769723827833</v>
+        <v>501.0262568474519</v>
       </c>
       <c r="J4" t="n">
-        <v>2.898747720188543</v>
+        <v>2.900304023139859</v>
       </c>
       <c r="K4" t="n">
-        <v>373.8351379084355</v>
+        <v>373.7607591608509</v>
       </c>
       <c r="L4" t="n">
-        <v>4.113282240343872</v>
+        <v>4.116154902120789</v>
       </c>
       <c r="M4" t="n">
-        <v>13.26658254372167</v>
+        <v>13.25378318244576</v>
       </c>
       <c r="N4" t="n">
-        <v>0.3480916912787412</v>
+        <v>0.3574245623082668</v>
       </c>
       <c r="O4" t="n">
-        <v>624.4827749838904</v>
+        <v>624.5813473946163</v>
       </c>
       <c r="P4" t="n">
-        <v>0.1466545503341509</v>
+        <v>0.1469303371178213</v>
       </c>
       <c r="Q4" t="n">
-        <v>8.582033034284141</v>
+        <v>8.231638550044488</v>
       </c>
       <c r="R4" t="n">
-        <v>188.2624846226897</v>
+        <v>186.5158304951203</v>
       </c>
       <c r="S4" t="n">
-        <v>22.24653288374755</v>
+        <v>20.79988349214914</v>
       </c>
       <c r="T4" t="n">
-        <v>19.82314256916902</v>
+        <v>18.72735885432487</v>
       </c>
     </row>
     <row r="5">
@@ -1642,13 +1642,13 @@
         <v>71</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.4117647058823529</v>
+        <v>-0.4444444444444444</v>
       </c>
       <c r="K6" t="n">
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.375</v>
+        <v>-0.4516129032258065</v>
       </c>
       <c r="M6" t="n">
         <v>1</v>
@@ -1700,7 +1700,7 @@
         <v>5374</v>
       </c>
       <c r="H7" t="n">
-        <v>0.05499999999999994</v>
+        <v>0.06113537117903922</v>
       </c>
       <c r="I7" t="n">
         <v>630</v>
@@ -1810,7 +1810,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>412</v>
+        <v>437</v>
       </c>
       <c r="C9" t="n">
         <v>141</v>
@@ -1825,31 +1825,31 @@
         <v>63</v>
       </c>
       <c r="G9" t="n">
-        <v>19690</v>
+        <v>19730</v>
       </c>
       <c r="H9" t="n">
         <v>10.3</v>
       </c>
       <c r="I9" t="n">
-        <v>1897</v>
+        <v>1833</v>
       </c>
       <c r="J9" t="n">
         <v>20</v>
       </c>
       <c r="K9" t="n">
-        <v>973</v>
+        <v>968</v>
       </c>
       <c r="L9" t="n">
         <v>34</v>
       </c>
       <c r="M9" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N9" t="n">
         <v>1</v>
       </c>
       <c r="O9" t="n">
-        <v>1777</v>
+        <v>1783</v>
       </c>
       <c r="P9" t="n">
         <v>0.8181818181818181</v>
@@ -1858,13 +1858,13 @@
         <v>35.51637279596977</v>
       </c>
       <c r="R9" t="n">
-        <v>889</v>
+        <v>831</v>
       </c>
       <c r="S9" t="n">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="T9" t="n">
-        <v>137</v>
+        <v>115.6666666666667</v>
       </c>
     </row>
     <row r="10">
@@ -1874,61 +1874,61 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>12734.31305309734</v>
+        <v>12907.58106826802</v>
       </c>
       <c r="C10" t="n">
-        <v>624.2580594184576</v>
+        <v>518.5488305941847</v>
       </c>
       <c r="D10" t="n">
-        <v>186.7220290771177</v>
+        <v>187.2656447534766</v>
       </c>
       <c r="E10" t="n">
-        <v>0.429993678887485</v>
+        <v>0.4265170670037928</v>
       </c>
       <c r="F10" t="n">
-        <v>357.3972819216182</v>
+        <v>361.7095448798987</v>
       </c>
       <c r="G10" t="n">
-        <v>39821768.79962075</v>
+        <v>39830901.71365359</v>
       </c>
       <c r="H10" t="n">
-        <v>1.396859438256318</v>
+        <v>1.39642434515441</v>
       </c>
       <c r="I10" t="n">
-        <v>252483.1077749684</v>
+        <v>251027.3100505688</v>
       </c>
       <c r="J10" t="n">
-        <v>8.402738345298276</v>
+        <v>8.411763426641249</v>
       </c>
       <c r="K10" t="n">
-        <v>139752.710335019</v>
+        <v>139697.1050884956</v>
       </c>
       <c r="L10" t="n">
-        <v>16.9190907887283</v>
+        <v>16.942731178253</v>
       </c>
       <c r="M10" t="n">
-        <v>176.0022123893806</v>
+        <v>175.6627686472821</v>
       </c>
       <c r="N10" t="n">
-        <v>0.1211678255372945</v>
+        <v>0.1277523177412561</v>
       </c>
       <c r="O10" t="n">
-        <v>389978.7362515802</v>
+        <v>390101.8595132743</v>
       </c>
       <c r="P10" t="n">
-        <v>0.021507557133712</v>
+        <v>0.02158852396555662</v>
       </c>
       <c r="Q10" t="n">
-        <v>73.65129100154425</v>
+        <v>67.75987321857853</v>
       </c>
       <c r="R10" t="n">
-        <v>35442.76311630848</v>
+        <v>34788.15502528445</v>
       </c>
       <c r="S10" t="n">
-        <v>494.9082253476612</v>
+        <v>432.6351532869784</v>
       </c>
       <c r="T10" t="n">
-        <v>392.9569813176008</v>
+        <v>350.7139696586599</v>
       </c>
     </row>
     <row r="11">
@@ -1938,61 +1938,61 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.07305108239002928</v>
+        <v>-0.03717091535261473</v>
       </c>
       <c r="C11" t="n">
-        <v>3.256948218980508</v>
+        <v>3.070847338950158</v>
       </c>
       <c r="D11" t="n">
-        <v>2.816819787633029</v>
+        <v>2.812340858379678</v>
       </c>
       <c r="E11" t="n">
-        <v>2.4787239858935</v>
+        <v>2.538777092501789</v>
       </c>
       <c r="F11" t="n">
-        <v>1.004449960762032</v>
+        <v>1.016662887922946</v>
       </c>
       <c r="G11" t="n">
-        <v>0.4661250842164482</v>
+        <v>0.4665028534278196</v>
       </c>
       <c r="H11" t="n">
-        <v>5.83036490346672</v>
+        <v>5.830884031568421</v>
       </c>
       <c r="I11" t="n">
-        <v>0.2811850588267728</v>
+        <v>0.2645771118129149</v>
       </c>
       <c r="J11" t="n">
-        <v>4.200222901005889</v>
+        <v>4.197054798204467</v>
       </c>
       <c r="K11" t="n">
-        <v>0.4615393087964401</v>
+        <v>0.4611637454660285</v>
       </c>
       <c r="L11" t="n">
-        <v>6.127265359226389</v>
+        <v>6.12028930948488</v>
       </c>
       <c r="M11" t="n">
-        <v>-0.02750040552113377</v>
+        <v>-0.02977201726454053</v>
       </c>
       <c r="N11" t="n">
-        <v>-1.605050125194589</v>
+        <v>-1.53986221140992</v>
       </c>
       <c r="O11" t="n">
-        <v>0.2191422605218263</v>
+        <v>0.2196656711853069</v>
       </c>
       <c r="P11" t="n">
-        <v>1.211300661628961</v>
+        <v>1.186308219243355</v>
       </c>
       <c r="Q11" t="n">
-        <v>1.373219134493004</v>
+        <v>1.296774111255319</v>
       </c>
       <c r="R11" t="n">
-        <v>0.7815775159089123</v>
+        <v>0.7147872094581595</v>
       </c>
       <c r="S11" t="n">
-        <v>3.448922639646042</v>
+        <v>3.104456278058441</v>
       </c>
       <c r="T11" t="n">
-        <v>3.352217164506285</v>
+        <v>2.915971394795704</v>
       </c>
     </row>
     <row r="12">
@@ -2002,61 +2002,61 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.9214196966297812</v>
+        <v>-0.848330652429476</v>
       </c>
       <c r="C12" t="n">
-        <v>12.89700509827747</v>
+        <v>12.50978422962784</v>
       </c>
       <c r="D12" t="n">
-        <v>10.71981759989129</v>
+        <v>10.6788640446567</v>
       </c>
       <c r="E12" t="n">
-        <v>6.443844325763778</v>
+        <v>6.729940528342262</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.4232329015640239</v>
+        <v>-0.3845585930454321</v>
       </c>
       <c r="G12" t="n">
-        <v>-1.200234167339935</v>
+        <v>-1.19921961817539</v>
       </c>
       <c r="H12" t="n">
-        <v>46.20784016624946</v>
+        <v>46.22028944142539</v>
       </c>
       <c r="I12" t="n">
-        <v>-1.04542328175748</v>
+        <v>-1.099597485232777</v>
       </c>
       <c r="J12" t="n">
-        <v>21.19592824065826</v>
+        <v>21.16829372368187</v>
       </c>
       <c r="K12" t="n">
-        <v>-1.578725079946602</v>
+        <v>-1.579633495745866</v>
       </c>
       <c r="L12" t="n">
-        <v>43.0348484892525</v>
+        <v>42.96111268603798</v>
       </c>
       <c r="M12" t="n">
-        <v>-1.791968360348134</v>
+        <v>-1.795450071989397</v>
       </c>
       <c r="N12" t="n">
-        <v>2.950330169705815</v>
+        <v>2.517934168007266</v>
       </c>
       <c r="O12" t="n">
-        <v>-1.684956307926789</v>
+        <v>-1.683660938549563</v>
       </c>
       <c r="P12" t="n">
-        <v>9.618070313763159</v>
+        <v>9.490959916065119</v>
       </c>
       <c r="Q12" t="n">
-        <v>1.482423746114138</v>
+        <v>1.287523141857604</v>
       </c>
       <c r="R12" t="n">
-        <v>0.4329201362761732</v>
+        <v>0.1182185947028573</v>
       </c>
       <c r="S12" t="n">
-        <v>15.45524400518077</v>
+        <v>12.8653949981309</v>
       </c>
       <c r="T12" t="n">
-        <v>15.65779300701639</v>
+        <v>11.59485905058041</v>
       </c>
     </row>
     <row r="13">
@@ -2066,61 +2066,61 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>95.8122014253271</v>
+        <v>96.1254600986766</v>
       </c>
       <c r="C13" t="n">
-        <v>15.94439658548046</v>
+        <v>15.18255149189443</v>
       </c>
       <c r="D13" t="n">
-        <v>9.360169159683609</v>
+        <v>9.386013000234946</v>
       </c>
       <c r="E13" t="n">
-        <v>0.4769363301746415</v>
+        <v>0.4686349753308789</v>
       </c>
       <c r="F13" t="n">
-        <v>15.99295167984962</v>
+        <v>16.06625420941342</v>
       </c>
       <c r="G13" t="n">
-        <v>5577.966168063271</v>
+        <v>5578.354608818232</v>
       </c>
       <c r="H13" t="n">
-        <v>0.6010605897226664</v>
+        <v>0.6005398070415311</v>
       </c>
       <c r="I13" t="n">
-        <v>450.085832876497</v>
+        <v>449.544521888949</v>
       </c>
       <c r="J13" t="n">
-        <v>1.584195892520544</v>
+        <v>1.586399811697586</v>
       </c>
       <c r="K13" t="n">
-        <v>349.0585010572477</v>
+        <v>349.006030229462</v>
       </c>
       <c r="L13" t="n">
-        <v>1.733504528204192</v>
+        <v>1.736323856264337</v>
       </c>
       <c r="M13" t="n">
-        <v>12.54428694494476</v>
+        <v>12.53551570209098</v>
       </c>
       <c r="N13" t="n">
-        <v>0.2332210823087162</v>
+        <v>0.2458558488004807</v>
       </c>
       <c r="O13" t="n">
-        <v>588.8948234004242</v>
+        <v>588.9502701856044</v>
       </c>
       <c r="P13" t="n">
-        <v>0.08227106172726516</v>
+        <v>0.08351188816686993</v>
       </c>
       <c r="Q13" t="n">
-        <v>6.743281871161313</v>
+        <v>6.538657360044938</v>
       </c>
       <c r="R13" t="n">
-        <v>147.2043229696922</v>
+        <v>146.586576865847</v>
       </c>
       <c r="S13" t="n">
-        <v>13.73929046910487</v>
+        <v>13.35680162894509</v>
       </c>
       <c r="T13" t="n">
-        <v>12.68708069021328</v>
+        <v>12.43647375153366</v>
       </c>
     </row>
   </sheetData>
@@ -9190,64 +9190,64 @@
     </row>
     <row r="114">
       <c r="A114" s="2" t="n">
-        <v>43998</v>
+        <v>43999</v>
       </c>
       <c r="B114" t="n">
-        <v>397</v>
+        <v>437</v>
       </c>
       <c r="C114" t="n">
-        <v>19690</v>
+        <v>19730</v>
       </c>
       <c r="D114" t="n">
-        <v>0</v>
+        <v>0.1007556675062973</v>
       </c>
       <c r="E114" t="n">
-        <v>141</v>
+        <v>77</v>
       </c>
       <c r="F114" t="n">
-        <v>1897</v>
+        <v>1833</v>
       </c>
       <c r="G114" t="n">
-        <v>0</v>
+        <v>-0.4539007092198581</v>
       </c>
       <c r="H114" t="n">
-        <v>141</v>
+        <v>109</v>
       </c>
       <c r="I114" t="n">
-        <v>137</v>
+        <v>115.6666666666667</v>
       </c>
       <c r="J114" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K114" t="n">
-        <v>973</v>
+        <v>968</v>
       </c>
       <c r="L114" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="M114" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N114" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O114" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="P114" t="n">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="Q114" t="n">
-        <v>1777</v>
+        <v>1783</v>
       </c>
       <c r="R114" t="n">
-        <v>0</v>
+        <v>0.1132075471698113</v>
       </c>
       <c r="S114" t="n">
-        <v>35.51637279596977</v>
+        <v>17.62013729977117</v>
       </c>
       <c r="T114" t="n">
-        <v>889</v>
+        <v>831</v>
       </c>
     </row>
   </sheetData>

</xml_diff>